<commit_message>
Add files via upload (#5)
надо решить проблему с else
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -409,7 +409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -430,26 +430,42 @@
           <t>dsffsdf</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fsdfsd</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>fd12321</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>realy&amp;</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>Arten</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>lol</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>/add_vendor</t>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gfdgfdg</t>
         </is>
       </c>
     </row>
@@ -459,11 +475,113 @@
           <t>None</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>добавь</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>/add_vendor</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>fdsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/add_vendor</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>u</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/addven</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>gfdgfdgfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>жив?</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>lol</t>
         </is>
       </c>
     </row>

</xml_diff>